<commit_message>
Sorting EPVs into sources corresponding to IDs. Adding linked alignments
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-refseqs-side-data.xlsx
@@ -148,8 +148,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="721">
+  <cellStyleXfs count="723">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -879,7 +881,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="721">
+  <cellStyles count="723">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1240,6 +1242,7 @@
     <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1600,6 +1603,7 @@
     <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1932,7 +1936,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Refactoring - creating valid EVE build
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50907891-807B-2F46-A0D6-95D04EF5C8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735FC931-B0C1-B04F-ABD9-BA6C7D33D049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>Xenarthra</t>
+  </si>
+  <si>
+    <t>Amdoparvovirus</t>
+  </si>
+  <si>
+    <t>amdo.2-ellobius</t>
+  </si>
+  <si>
+    <t>amdo.1-ellobius</t>
   </si>
 </sst>
 </file>
@@ -206,18 +215,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFADFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -228,6 +231,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBAD8E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,25 +981,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="723">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1715,6 +1735,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FDFF"/>
       <color rgb="FFBAD8E8"/>
     </mruColors>
   </colors>
@@ -2051,16 +2072,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="A1:M11"/>
+      <selection activeCell="E10" sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
@@ -2073,407 +2094,480 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1"/>
+      <c r="J2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="9">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="E3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="7">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="7">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="H5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="7">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="A6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="1"/>
+      <c r="I6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="7">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="D7" s="10">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="E7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="1"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="7">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="A8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="11">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="1"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="7">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="D9" s="10">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="I9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M9" s="1"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="11">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="D10" s="10">
+        <v>11</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="H10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="8">
+      <c r="A11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="11">
+        <v>12</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="10">
+        <v>12</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="H11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="D12" s="10">
+        <v>13</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="H12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="11">
+        <v>13</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="10">
+        <v>13</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="10"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M13">
+    <sortCondition ref="H2:H13"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>